<commit_message>
[Work] Config Excel File Basic Work
- Sheet 구성 완료.
</commit_message>
<xml_diff>
--- a/Solving_Sdoku/Win32/Debug/Config/Config.xlsx
+++ b/Solving_Sdoku/Win32/Debug/Config/Config.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\01. MJW\01. Project\01. Game\SolvingSdoku\010_Source\Solving_Sdoku\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\01. MJW\01. Project\01. Game\SolvingSdoku\010_Source\Solving_Sdoku\Win32\Debug\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{104B7D99-9703-42F2-BB87-05286BA7C1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C2F33D-0538-401C-BBB9-9A8D492B8BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F0E7DE0A-5F33-4E6C-909F-CE2C96A94F8A}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{F0E7DE0A-5F33-4E6C-909F-CE2C96A94F8A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="readme" sheetId="1" r:id="rId1"/>
+    <sheet name="Solver" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,6 +31,27 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Idx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 본 엑셀파일을 저장 후 프로그램을 실행하세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Solver Sheet 에 해결하고 싶은 스도쿠 문제를 입력하세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 프로그램 실행 후 Solver 페이지로 이동하여 문제 풀이를 진행하세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -51,15 +73,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -67,15 +101,215 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -391,12 +625,216 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA359B3-D11E-4DA9-A571-8D7C170B04FF}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{827A47F8-A527-491E-9158-86B9B338098C}">
+  <dimension ref="B2:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="5.625" style="1" customWidth="1"/>
+    <col min="3" max="11" width="10.625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3">
+        <v>4</v>
+      </c>
+      <c r="H2" s="3">
+        <v>5</v>
+      </c>
+      <c r="I2" s="3">
+        <v>6</v>
+      </c>
+      <c r="J2" s="3">
+        <v>7</v>
+      </c>
+      <c r="K2" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="2:11" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="4">
+        <v>2</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="13"/>
+    </row>
+    <row r="6" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="4">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="4">
+        <v>4</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="2:11" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="4">
+        <v>5</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="13"/>
+    </row>
+    <row r="9" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="4">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="4">
+        <v>7</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" spans="2:11" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="4">
+        <v>8</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="13">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[Test] Load Sheet Test
</commit_message>
<xml_diff>
--- a/Solving_Sdoku/Win32/Debug/Config/Config.xlsx
+++ b/Solving_Sdoku/Win32/Debug/Config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\01. MJW\01. Project\01. Game\SolvingSdoku\010_Source\Solving_Sdoku\Win32\Debug\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C2F33D-0538-401C-BBB9-9A8D492B8BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC938C3-49DF-4C75-9B57-46D650541119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{F0E7DE0A-5F33-4E6C-909F-CE2C96A94F8A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F0E7DE0A-5F33-4E6C-909F-CE2C96A94F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +67,23 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -268,7 +285,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -284,31 +301,34 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -659,20 +679,58 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{827A47F8-A527-491E-9158-86B9B338098C}">
-  <dimension ref="B2:K11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="1" max="1" width="2.625" style="14" customWidth="1"/>
     <col min="2" max="2" width="5.625" style="1" customWidth="1"/>
     <col min="3" max="11" width="10.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14">
+        <v>2</v>
+      </c>
+      <c r="D1" s="14">
+        <v>3</v>
+      </c>
+      <c r="E1" s="14">
+        <v>4</v>
+      </c>
+      <c r="F1" s="14">
+        <v>5</v>
+      </c>
+      <c r="G1" s="14">
+        <v>6</v>
+      </c>
+      <c r="H1" s="14">
+        <v>7</v>
+      </c>
+      <c r="I1" s="14">
+        <v>8</v>
+      </c>
+      <c r="J1" s="14">
+        <v>9</v>
+      </c>
+      <c r="K1" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -704,7 +762,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14">
+        <v>2</v>
+      </c>
       <c r="B3" s="4">
         <v>0</v>
       </c>
@@ -713,42 +774,67 @@
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="5"/>
+      <c r="F3" s="5">
+        <v>4</v>
+      </c>
       <c r="G3" s="6"/>
       <c r="H3" s="7"/>
-      <c r="I3" s="5"/>
+      <c r="I3" s="5">
+        <v>7</v>
+      </c>
       <c r="J3" s="6"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14">
+        <v>3</v>
+      </c>
       <c r="B4" s="4">
         <v>1</v>
       </c>
       <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
+      <c r="D4" s="9">
+        <v>2</v>
+      </c>
       <c r="E4" s="10"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="9"/>
+      <c r="G4" s="9">
+        <v>5</v>
+      </c>
       <c r="H4" s="10"/>
       <c r="I4" s="8"/>
-      <c r="J4" s="9"/>
+      <c r="J4" s="9">
+        <v>8</v>
+      </c>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="2:11" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="14">
+        <v>4</v>
+      </c>
       <c r="B5" s="4">
         <v>2</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
+      <c r="E5" s="13">
+        <v>3</v>
+      </c>
       <c r="F5" s="11"/>
       <c r="G5" s="12"/>
-      <c r="H5" s="13"/>
+      <c r="H5" s="13">
+        <v>6</v>
+      </c>
       <c r="I5" s="11"/>
       <c r="J5" s="12"/>
-      <c r="K5" s="13"/>
-    </row>
-    <row r="6" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K5" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14">
+        <v>5</v>
+      </c>
       <c r="B6" s="4">
         <v>3</v>
       </c>
@@ -762,7 +848,10 @@
       <c r="J6" s="6"/>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14">
+        <v>6</v>
+      </c>
       <c r="B7" s="4">
         <v>4</v>
       </c>
@@ -776,7 +865,10 @@
       <c r="J7" s="9"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="2:11" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14">
+        <v>7</v>
+      </c>
       <c r="B8" s="4">
         <v>5</v>
       </c>
@@ -790,52 +882,78 @@
       <c r="J8" s="12"/>
       <c r="K8" s="13"/>
     </row>
-    <row r="9" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
+        <v>8</v>
+      </c>
       <c r="B9" s="4">
         <v>6</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="5">
+        <v>7</v>
+      </c>
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
       <c r="G9" s="6"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="5"/>
+      <c r="I9" s="5">
+        <v>4</v>
+      </c>
       <c r="J9" s="6"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="14">
+        <v>9</v>
+      </c>
       <c r="B10" s="4">
         <v>7</v>
       </c>
       <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
+      <c r="D10" s="9">
+        <v>8</v>
+      </c>
       <c r="E10" s="10"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="9"/>
+      <c r="G10" s="9">
+        <v>2</v>
+      </c>
       <c r="H10" s="10"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="9"/>
+      <c r="J10" s="9">
+        <v>5</v>
+      </c>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="2:11" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="14">
+        <v>10</v>
+      </c>
       <c r="B11" s="4">
         <v>8</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
+      <c r="E11" s="13">
+        <v>9</v>
+      </c>
       <c r="F11" s="11"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="13"/>
+      <c r="H11" s="13">
+        <v>3</v>
+      </c>
       <c r="I11" s="11"/>
       <c r="J11" s="12"/>
       <c r="K11" s="13">
-        <v>81</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[memo] Pause ( Error )
- error occurred. I don't know why yet.
</commit_message>
<xml_diff>
--- a/Solving_Sdoku/Win32/Debug/Config/Config.xlsx
+++ b/Solving_Sdoku/Win32/Debug/Config/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\01. MJW\01. Project\01. Game\SolvingSdoku\010_Source\Solving_Sdoku\Win32\Debug\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC938C3-49DF-4C75-9B57-46D650541119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E611C146-51DB-452A-85C9-F2844F7D982E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F0E7DE0A-5F33-4E6C-909F-CE2C96A94F8A}"/>
   </bookViews>
@@ -682,7 +682,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -774,14 +774,10 @@
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="5">
-        <v>4</v>
-      </c>
+      <c r="F3" s="5"/>
       <c r="G3" s="6"/>
       <c r="H3" s="7"/>
-      <c r="I3" s="5">
-        <v>7</v>
-      </c>
+      <c r="I3" s="5"/>
       <c r="J3" s="6"/>
       <c r="K3" s="7"/>
     </row>
@@ -793,19 +789,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="8"/>
-      <c r="D4" s="9">
-        <v>2</v>
-      </c>
+      <c r="D4" s="9"/>
       <c r="E4" s="10"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="9">
-        <v>5</v>
-      </c>
+      <c r="G4" s="9"/>
       <c r="H4" s="10"/>
       <c r="I4" s="8"/>
-      <c r="J4" s="9">
-        <v>8</v>
-      </c>
+      <c r="J4" s="9"/>
       <c r="K4" s="10"/>
     </row>
     <row r="5" spans="1:11" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -817,19 +807,13 @@
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="12"/>
-      <c r="E5" s="13">
-        <v>3</v>
-      </c>
+      <c r="E5" s="13"/>
       <c r="F5" s="11"/>
       <c r="G5" s="12"/>
-      <c r="H5" s="13">
-        <v>6</v>
-      </c>
+      <c r="H5" s="13"/>
       <c r="I5" s="11"/>
       <c r="J5" s="12"/>
-      <c r="K5" s="13">
-        <v>9</v>
-      </c>
+      <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
@@ -889,19 +873,13 @@
       <c r="B9" s="4">
         <v>6</v>
       </c>
-      <c r="C9" s="5">
-        <v>7</v>
-      </c>
+      <c r="C9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
-      <c r="F9" s="5">
-        <v>1</v>
-      </c>
+      <c r="F9" s="5"/>
       <c r="G9" s="6"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="5">
-        <v>4</v>
-      </c>
+      <c r="I9" s="5"/>
       <c r="J9" s="6"/>
       <c r="K9" s="7"/>
     </row>
@@ -913,19 +891,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="8"/>
-      <c r="D10" s="9">
-        <v>8</v>
-      </c>
+      <c r="D10" s="9"/>
       <c r="E10" s="10"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="9">
-        <v>2</v>
-      </c>
+      <c r="G10" s="9"/>
       <c r="H10" s="10"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="9">
-        <v>5</v>
-      </c>
+      <c r="J10" s="9"/>
       <c r="K10" s="10"/>
     </row>
     <row r="11" spans="1:11" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -937,19 +909,13 @@
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="13">
-        <v>9</v>
-      </c>
+      <c r="E11" s="13"/>
       <c r="F11" s="11"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="13">
-        <v>3</v>
-      </c>
+      <c r="H11" s="13"/>
       <c r="I11" s="11"/>
       <c r="J11" s="12"/>
-      <c r="K11" s="13">
-        <v>6</v>
-      </c>
+      <c r="K11" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
[Test] Expert Mode Fail...
- 아무리 기다려도 안나오네.. 뭔가 방법을 바꾸어 봐야할듯.
</commit_message>
<xml_diff>
--- a/Solving_Sdoku/Win32/Debug/Config/Config.xlsx
+++ b/Solving_Sdoku/Win32/Debug/Config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\01. MJW\01. Project\01. Game\SolvingSdoku\010_Source\Solving_Sdoku\Win32\Debug\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E611C146-51DB-452A-85C9-F2844F7D982E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D7B74F-926C-4587-93AD-B190BE5676AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F0E7DE0A-5F33-4E6C-909F-CE2C96A94F8A}"/>
+    <workbookView xWindow="4560" yWindow="7650" windowWidth="28800" windowHeight="14190" activeTab="1" xr2:uid="{F0E7DE0A-5F33-4E6C-909F-CE2C96A94F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
@@ -682,7 +682,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -769,17 +769,21 @@
       <c r="B3" s="4">
         <v>0</v>
       </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
+      <c r="C3" s="5"/>
       <c r="D3" s="6"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="5"/>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
       <c r="G3" s="6"/>
       <c r="H3" s="7"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="7"/>
+      <c r="J3" s="6">
+        <v>3</v>
+      </c>
+      <c r="K3" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14">
@@ -790,12 +794,18 @@
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="10"/>
+      <c r="E4" s="10">
+        <v>5</v>
+      </c>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
+      <c r="H4" s="10">
+        <v>3</v>
+      </c>
       <c r="I4" s="8"/>
-      <c r="J4" s="9"/>
+      <c r="J4" s="9">
+        <v>9</v>
+      </c>
       <c r="K4" s="10"/>
     </row>
     <row r="5" spans="1:11" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -810,7 +820,9 @@
       <c r="E5" s="13"/>
       <c r="F5" s="11"/>
       <c r="G5" s="12"/>
-      <c r="H5" s="13"/>
+      <c r="H5" s="13">
+        <v>2</v>
+      </c>
       <c r="I5" s="11"/>
       <c r="J5" s="12"/>
       <c r="K5" s="13"/>
@@ -824,13 +836,17 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
+      <c r="E6" s="7">
+        <v>6</v>
+      </c>
       <c r="F6" s="5"/>
       <c r="G6" s="6"/>
       <c r="H6" s="7"/>
       <c r="I6" s="5"/>
       <c r="J6" s="6"/>
-      <c r="K6" s="7"/>
+      <c r="K6" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
@@ -842,10 +858,16 @@
       <c r="C7" s="8"/>
       <c r="D7" s="9"/>
       <c r="E7" s="10"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9"/>
+      <c r="F7" s="8">
+        <v>6</v>
+      </c>
+      <c r="G7" s="9">
+        <v>4</v>
+      </c>
       <c r="H7" s="10"/>
-      <c r="I7" s="8"/>
+      <c r="I7" s="8">
+        <v>7</v>
+      </c>
       <c r="J7" s="9"/>
       <c r="K7" s="10"/>
     </row>
@@ -856,13 +878,17 @@
       <c r="B8" s="4">
         <v>5</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="11">
+        <v>9</v>
+      </c>
       <c r="D8" s="12"/>
       <c r="E8" s="13"/>
       <c r="F8" s="11"/>
       <c r="G8" s="12"/>
       <c r="H8" s="13"/>
-      <c r="I8" s="11"/>
+      <c r="I8" s="11">
+        <v>5</v>
+      </c>
       <c r="J8" s="12"/>
       <c r="K8" s="13"/>
     </row>
@@ -873,9 +899,15 @@
       <c r="B9" s="4">
         <v>6</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6">
+        <v>3</v>
+      </c>
+      <c r="E9" s="7">
+        <v>9</v>
+      </c>
       <c r="F9" s="5"/>
       <c r="G9" s="6"/>
       <c r="H9" s="7"/>
@@ -891,11 +923,17 @@
         <v>7</v>
       </c>
       <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
+      <c r="D10" s="9">
+        <v>5</v>
+      </c>
       <c r="E10" s="10"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="10"/>
+      <c r="G10" s="9">
+        <v>1</v>
+      </c>
+      <c r="H10" s="10">
+        <v>7</v>
+      </c>
       <c r="I10" s="8"/>
       <c r="J10" s="9"/>
       <c r="K10" s="10"/>
@@ -908,10 +946,14 @@
         <v>8</v>
       </c>
       <c r="C11" s="11"/>
-      <c r="D11" s="12"/>
+      <c r="D11" s="12">
+        <v>1</v>
+      </c>
       <c r="E11" s="13"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
+      <c r="G11" s="12">
+        <v>8</v>
+      </c>
       <c r="H11" s="13"/>
       <c r="I11" s="11"/>
       <c r="J11" s="12"/>

</xml_diff>